<commit_message>
bara eitthvad ad fikta i thessu
</commit_message>
<xml_diff>
--- a/Verkefni1/Gistingar_larus.xlsx
+++ b/Verkefni1/Gistingar_larus.xlsx
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20775" windowHeight="11445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20775" windowHeight="11445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gistingar" sheetId="1" r:id="rId1"/>
     <sheet name="Unnið" sheetId="2" r:id="rId2"/>
+    <sheet name="Forsendur" sheetId="3" r:id="rId3"/>
+    <sheet name="Hugmynd 1" sheetId="4" r:id="rId4"/>
+    <sheet name="Hugmynd 2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="64">
   <si>
     <t>Gistinætur á hótelum 1997-2014</t>
   </si>
@@ -122,13 +125,106 @@
   </si>
   <si>
     <t>..</t>
+  </si>
+  <si>
+    <t>Þarf að g.r.f. Eðlilegum árlegum vexti</t>
+  </si>
+  <si>
+    <t>Airwaves byrjaði 1999</t>
+  </si>
+  <si>
+    <t>Hátíðin er 5 daga, miðvikudag til sunnudags, á tímabilinu frá miðjum okt fram í miðjan nóv</t>
+  </si>
+  <si>
+    <t>14-18 okt</t>
+  </si>
+  <si>
+    <t>13-17 okt</t>
+  </si>
+  <si>
+    <t>12-17 okt</t>
+  </si>
+  <si>
+    <t>31 okt - 4 nóv</t>
+  </si>
+  <si>
+    <t>30 okt - 3 nóv</t>
+  </si>
+  <si>
+    <t>Berum saman vöxt í gistinóttum í október og nóvember frá 1999 vs meðalvöxt í öðrum mánuðum</t>
+  </si>
+  <si>
+    <t>Meðalvöxtur utan okt-nóv</t>
+  </si>
+  <si>
+    <t>Erum ekki með gögn fyrir gistinæstur í okt-nóv 2014 þannig við sleppum því ári</t>
+  </si>
+  <si>
+    <t>Iceland Airwaves byrjaði 1999 svo við skoðum ekki lengra aftur í tímann</t>
+  </si>
+  <si>
+    <t>Meðalvöxtur okt-nóv</t>
+  </si>
+  <si>
+    <t>Allt tímabil</t>
+  </si>
+  <si>
+    <t>1999-2004</t>
+  </si>
+  <si>
+    <t>2005-2009</t>
+  </si>
+  <si>
+    <t>2010-2013</t>
+  </si>
+  <si>
+    <t>Hugmynd 2</t>
+  </si>
+  <si>
+    <t>Hugmynd 1</t>
+  </si>
+  <si>
+    <t>Skoða hvort að okt-nóv verða stækki meira hlutfallslega en hinir mánuðir ársins</t>
+  </si>
+  <si>
+    <t>Okt+nóv af heildargistinóttum árs</t>
+  </si>
+  <si>
+    <t>hlutfall okt+nóv af árinu hefur ekki breyst að neinu marki</t>
+  </si>
+  <si>
+    <t>http://www.vb.is/frettir/81922/</t>
+  </si>
+  <si>
+    <t>Hugmynd 3</t>
+  </si>
+  <si>
+    <t>Skoða okt vs nóv, þ.e. skoða airwaves mánuðinn á móti hinum mánuðinum þar sem hátíðin er haldin sitt á hvað í okt og nóv, sjá vb frétt</t>
+  </si>
+  <si>
+    <t>http://www.uton.is/wp-content/uploads/2012/01/SK%C3%9DRSLA_ICELANDAIRWAVES_2011.pdf</t>
+  </si>
+  <si>
+    <t>Hugmynd 4</t>
+  </si>
+  <si>
+    <t>Skoða ársfjórðunga</t>
+  </si>
+  <si>
+    <t>http://www.m5.is/?gluggi=frett&amp;id=186048</t>
+  </si>
+  <si>
+    <t>http://www.landsbankinn.is/uploads/documents/frettir/Ferdathjonusta-a-Islandi-Greining.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +233,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -190,10 +294,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -210,9 +315,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1906,11 +2016,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,4 +2822,574 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2009</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2010</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2011</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2012</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2013</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2013</v>
+      </c>
+      <c r="C3" s="7">
+        <f>(SUM(Unnið!C5:K5)+Unnið!N5)/(SUM(Unnið!C6:K6)+Unnið!N6) - 1</f>
+        <v>0.10221402109374789</v>
+      </c>
+      <c r="D3" s="7">
+        <f>(Unnið!L5+Unnið!M5)/(Unnið!L6+Unnið!M6) - 1</f>
+        <v>0.17004520001270262</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2012</v>
+      </c>
+      <c r="C4" s="7">
+        <f>(SUM(Unnið!C6:K6)+Unnið!N6)/(SUM(Unnið!C7:K7)+Unnið!N7) - 1</f>
+        <v>0.19327362353498545</v>
+      </c>
+      <c r="D4" s="7">
+        <f>(Unnið!L6+Unnið!M6)/(Unnið!L7+Unnið!M7) - 1</f>
+        <v>0.26289545275287929</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2011</v>
+      </c>
+      <c r="C5" s="7">
+        <f>(SUM(Unnið!C7:K7)+Unnið!N7)/(SUM(Unnið!C8:K8)+Unnið!N8) - 1</f>
+        <v>0.17086204323357679</v>
+      </c>
+      <c r="D5" s="7">
+        <f>(Unnið!L7+Unnið!M7)/(Unnið!L8+Unnið!M8) - 1</f>
+        <v>0.16086005152239369</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2010</v>
+      </c>
+      <c r="C6" s="7">
+        <f>(SUM(Unnið!C8:K8)+Unnið!N8)/(SUM(Unnið!C9:K9)+Unnið!N9) - 1</f>
+        <v>-1.7261520010591336E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <f>(Unnið!L8+Unnið!M8)/(Unnið!L9+Unnið!M9) - 1</f>
+        <v>-5.453745139754973E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2009</v>
+      </c>
+      <c r="C7" s="7">
+        <f>(SUM(Unnið!C9:K9)+Unnið!N9)/(SUM(Unnið!C10:K10)+Unnið!N10) - 1</f>
+        <v>-6.0326298705487558E-3</v>
+      </c>
+      <c r="D7" s="7">
+        <f>(Unnið!L9+Unnið!M9)/(Unnið!L10+Unnið!M10) - 1</f>
+        <v>-1.2045922361058725E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2008</v>
+      </c>
+      <c r="C8" s="7">
+        <f>(SUM(Unnið!C10:K10)+Unnið!N10)/(SUM(Unnið!C11:K11)+Unnið!N11) - 1</f>
+        <v>2.9851856772736385E-2</v>
+      </c>
+      <c r="D8" s="7">
+        <f>(Unnið!L10+Unnið!M10)/(Unnið!L11+Unnið!M11) - 1</f>
+        <v>-3.640744491392256E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2007</v>
+      </c>
+      <c r="C9" s="7">
+        <f>(SUM(Unnið!C11:K11)+Unnið!N11)/(SUM(Unnið!C12:K12)+Unnið!N12) - 1</f>
+        <v>0.13931715144221668</v>
+      </c>
+      <c r="D9" s="7">
+        <f>(Unnið!L11+Unnið!M11)/(Unnið!L12+Unnið!M12) - 1</f>
+        <v>0.13182565529452672</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2006</v>
+      </c>
+      <c r="C10" s="7">
+        <f>(SUM(Unnið!C12:K12)+Unnið!N12)/(SUM(Unnið!C13:K13)+Unnið!N13) - 1</f>
+        <v>0.10617609334132605</v>
+      </c>
+      <c r="D10" s="7">
+        <f>(Unnið!L12+Unnið!M12)/(Unnið!L13+Unnið!M13) - 1</f>
+        <v>0.21139114447678864</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2005</v>
+      </c>
+      <c r="C11" s="7">
+        <f>(SUM(Unnið!C13:K13)+Unnið!N13)/(SUM(Unnið!C14:K14)+Unnið!N14) - 1</f>
+        <v>8.3027004676990313E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <f>(Unnið!L13+Unnið!M13)/(Unnið!L14+Unnið!M14) - 1</f>
+        <v>4.6368446368445504E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2004</v>
+      </c>
+      <c r="C12" s="7">
+        <f>(SUM(Unnið!C14:K14)+Unnið!N14)/(SUM(Unnið!C15:K15)+Unnið!N15) - 1</f>
+        <v>9.4747061240939567E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <f>(Unnið!L14+Unnið!M14)/(Unnið!L15+Unnið!M15) - 1</f>
+        <v>9.2692259176722969E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2003</v>
+      </c>
+      <c r="C13" s="7">
+        <f>(SUM(Unnið!C15:K15)+Unnið!N15)/(SUM(Unnið!C16:K16)+Unnið!N16) - 1</f>
+        <v>7.4340133732896829E-2</v>
+      </c>
+      <c r="D13" s="7">
+        <f>(Unnið!L15+Unnið!M15)/(Unnið!L16+Unnið!M16) - 1</f>
+        <v>0.20886968676535989</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2002</v>
+      </c>
+      <c r="C14" s="7">
+        <f>(SUM(Unnið!C16:K16)+Unnið!N16)/(SUM(Unnið!C17:K17)+Unnið!N17) - 1</f>
+        <v>3.2893896200601791E-2</v>
+      </c>
+      <c r="D14" s="7">
+        <f>(Unnið!L16+Unnið!M16)/(Unnið!L17+Unnið!M17) - 1</f>
+        <v>-4.8232405694036307E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2001</v>
+      </c>
+      <c r="C15" s="7">
+        <f>(SUM(Unnið!C17:K17)+Unnið!N17)/(SUM(Unnið!C18:K18)+Unnið!N18) - 1</f>
+        <v>1.2554485306255359E-2</v>
+      </c>
+      <c r="D15" s="7">
+        <f>(Unnið!L17+Unnið!M17)/(Unnið!L18+Unnið!M18) - 1</f>
+        <v>1.4814178408365741E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2000</v>
+      </c>
+      <c r="C16" s="7">
+        <f>(SUM(Unnið!C18:K18)+Unnið!N18)/(SUM(Unnið!C19:K19)+Unnið!N19) - 1</f>
+        <v>5.6595501963353945E-2</v>
+      </c>
+      <c r="D16" s="7">
+        <f>(Unnið!L18+Unnið!M18)/(Unnið!L19+Unnið!M19) - 1</f>
+        <v>7.2631287931647304E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1999</v>
+      </c>
+      <c r="C17" s="7">
+        <f>(SUM(Unnið!C19:K19)+Unnið!N19)/(SUM(Unnið!C20:K20)+Unnið!N20) - 1</f>
+        <v>8.7912736000246072E-2</v>
+      </c>
+      <c r="D17" s="7">
+        <f>(Unnið!L19+Unnið!M19)/(Unnið!L20+Unnið!M20) - 1</f>
+        <v>5.9710654445513933E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="9">
+        <f>AVERAGE(C3:C17)</f>
+        <v>7.7364763910582196E-2</v>
+      </c>
+      <c r="D19" s="9">
+        <f>AVERAGE(D3:D17)</f>
+        <v>8.2609946070478543E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="8">
+        <f>AVERAGE(C13:C17)</f>
+        <v>5.2859350640670801E-2</v>
+      </c>
+      <c r="D21" s="8">
+        <f>AVERAGE(D13:D17)</f>
+        <v>6.1558680371370113E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="8">
+        <f>AVERAGE(C7:C11)</f>
+        <v>7.0467895272544129E-2</v>
+      </c>
+      <c r="D22" s="8">
+        <f>AVERAGE(D7:D11)</f>
+        <v>5.9880055426635728E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="8">
+        <f>AVERAGE(C2:C6)</f>
+        <v>0.1122720419629297</v>
+      </c>
+      <c r="D23" s="8">
+        <f>AVERAGE(D2:D6)</f>
+        <v>0.13481581322260647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2013</v>
+      </c>
+      <c r="C3" s="10">
+        <f>(Unnið!L5+Unnið!M5)/SUM(Unnið!C5:N5)</f>
+        <v>0.15937945642597701</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2012</v>
+      </c>
+      <c r="C4" s="10">
+        <f>(Unnið!L6+Unnið!M6)/SUM(Unnið!C6:N6)</f>
+        <v>0.15153991820575607</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2011</v>
+      </c>
+      <c r="C5" s="10">
+        <f>(Unnið!L7+Unnið!M7)/SUM(Unnið!C7:N7)</f>
+        <v>0.1443919943404075</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2010</v>
+      </c>
+      <c r="C6" s="10">
+        <f>(Unnið!L8+Unnið!M8)/SUM(Unnið!C8:N8)</f>
+        <v>0.14545512003692923</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2009</v>
+      </c>
+      <c r="C7" s="10">
+        <f>(Unnið!L9+Unnið!M9)/SUM(Unnið!C9:N9)</f>
+        <v>0.15032776326933936</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2008</v>
+      </c>
+      <c r="C8" s="10">
+        <f>(Unnið!L10+Unnið!M10)/SUM(Unnið!C10:N10)</f>
+        <v>0.15110449134258397</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2007</v>
+      </c>
+      <c r="C9" s="10">
+        <f>(Unnið!L11+Unnið!M11)/SUM(Unnið!C11:N11)</f>
+        <v>0.15983412123884422</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2006</v>
+      </c>
+      <c r="C10" s="10">
+        <f>(Unnið!L12+Unnið!M12)/SUM(Unnið!C12:N12)</f>
+        <v>0.16072202184410822</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2005</v>
+      </c>
+      <c r="C11" s="10">
+        <f>(Unnið!L13+Unnið!M13)/SUM(Unnið!C13:N13)</f>
+        <v>0.14884028516129399</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2004</v>
+      </c>
+      <c r="C12" s="10">
+        <f>(Unnið!L14+Unnið!M14)/SUM(Unnið!C14:N14)</f>
+        <v>0.15861196601019573</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2003</v>
+      </c>
+      <c r="C13" s="10">
+        <f>(Unnið!L15+Unnið!M15)/SUM(Unnið!C15:N15)</f>
+        <v>0.15886285112160192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2002</v>
+      </c>
+      <c r="C14" s="10">
+        <f>(Unnið!L16+Unnið!M16)/SUM(Unnið!C16:N16)</f>
+        <v>0.14372465938561566</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2001</v>
+      </c>
+      <c r="C15" s="10">
+        <f>(Unnið!L17+Unnið!M17)/SUM(Unnið!C17:N17)</f>
+        <v>0.15408770455295129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2000</v>
+      </c>
+      <c r="C16" s="10">
+        <f>(Unnið!L18+Unnið!M18)/SUM(Unnið!C18:N18)</f>
+        <v>0.15379736560946236</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1999</v>
+      </c>
+      <c r="C17" s="10">
+        <f>(Unnið!L19+Unnið!M19)/SUM(Unnið!C19:N19)</f>
+        <v>0.15184723918653908</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bjo til geggjad shit, speccidi thad vid tækifæri
</commit_message>
<xml_diff>
--- a/Verkefni1/Gistingar_larus.xlsx
+++ b/Verkefni1/Gistingar_larus.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="67">
   <si>
     <t>Gistinætur á hótelum 1997-2014</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t>http://www.landsbankinn.is/uploads/documents/frettir/Ferdathjonusta-a-Islandi-Greining.pdf</t>
+  </si>
+  <si>
+    <t>Eftir spjall við Eyjólf:</t>
+  </si>
+  <si>
+    <t>Setja upp graf fyrir gistinætur sem fall af mánuðum, sjá hvort trendið breytist yfir árin, sérstaklega fyrir okt-nóv</t>
+  </si>
+  <si>
+    <t>Bera saman sept-okt-nóv-des eftir árum, sjá hvort við sjáum mun á vexti</t>
   </si>
 </sst>
 </file>
@@ -2826,10 +2835,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D21"/>
+  <dimension ref="A3:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2952,6 +2961,19 @@
       </c>
       <c r="B21" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>